<commit_message>
modified hospital screens to add navigation
modified hospital screens to add navigation
</commit_message>
<xml_diff>
--- a/Login Users.xlsx
+++ b/Login Users.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC1048F5A1DA4F8A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC69076-2FE2-43C6-8045-A1C8A72475D7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3893" yWindow="3697" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="C4:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
changes done in screen to fix navigations
changes done in screen to fix navigations
</commit_message>
<xml_diff>
--- a/Login Users.xlsx
+++ b/Login Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cba81a96ab6550d/Documents/GitHub/Final_project_AED_Spr2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC1048F5A1DA4F8A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC69076-2FE2-43C6-8045-A1C8A72475D7}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="11_F25DC773A252ABDACC1048F5A1DA4F8A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{668D8C05-0476-4914-A842-500227A1C7CF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3893" yWindow="3697" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3893" yWindow="3697" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>FR_user12345</t>
+  </si>
+  <si>
+    <t>BB_user</t>
+  </si>
+  <si>
+    <t>BB_user12345</t>
+  </si>
+  <si>
+    <t>Blood Bank</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -193,14 +202,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:E15"/>
+  <dimension ref="C4:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -626,6 +647,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
UI layout changes for button and screen colour
UI layout changes for button and screen colour
</commit_message>
<xml_diff>
--- a/Login Users.xlsx
+++ b/Login Users.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="71" documentId="11_F25DC773A252ABDACC1048F5A1DA4F8A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{668D8C05-0476-4914-A842-500227A1C7CF}"/>
   <bookViews>
-    <workbookView xWindow="3893" yWindow="3697" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3893" yWindow="3697" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="C4:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>